<commit_message>
Exam Center Final changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Files/ControllerTemplate .xlsx
+++ b/src/test/resources/Files/ControllerTemplate .xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="2877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3005" uniqueCount="2997">
   <si>
     <t>FirstName</t>
   </si>
@@ -8650,6 +8650,366 @@
   </si>
   <si>
     <t>97572</t>
+  </si>
+  <si>
+    <t>Controller12927</t>
+  </si>
+  <si>
+    <t>Automation12927</t>
+  </si>
+  <si>
+    <t>controllerautomation12927@gmail.com</t>
+  </si>
+  <si>
+    <t>12927</t>
+  </si>
+  <si>
+    <t>Controller40980</t>
+  </si>
+  <si>
+    <t>Automation40980</t>
+  </si>
+  <si>
+    <t>controllerautomation40980@gmail.com</t>
+  </si>
+  <si>
+    <t>40980</t>
+  </si>
+  <si>
+    <t>Controller42031</t>
+  </si>
+  <si>
+    <t>Automation42031</t>
+  </si>
+  <si>
+    <t>controllerautomation42031@gmail.com</t>
+  </si>
+  <si>
+    <t>42031</t>
+  </si>
+  <si>
+    <t>Controller00433</t>
+  </si>
+  <si>
+    <t>Automation00433</t>
+  </si>
+  <si>
+    <t>controllerautomation00433@gmail.com</t>
+  </si>
+  <si>
+    <t>00433</t>
+  </si>
+  <si>
+    <t>Controller74772</t>
+  </si>
+  <si>
+    <t>Automation74772</t>
+  </si>
+  <si>
+    <t>controllerautomation74772@gmail.com</t>
+  </si>
+  <si>
+    <t>74772</t>
+  </si>
+  <si>
+    <t>Controller32431</t>
+  </si>
+  <si>
+    <t>Automation32431</t>
+  </si>
+  <si>
+    <t>controllerautomation32431@gmail.com</t>
+  </si>
+  <si>
+    <t>32431</t>
+  </si>
+  <si>
+    <t>Controller59839</t>
+  </si>
+  <si>
+    <t>Automation59839</t>
+  </si>
+  <si>
+    <t>controllerautomation59839@gmail.com</t>
+  </si>
+  <si>
+    <t>59839</t>
+  </si>
+  <si>
+    <t>Controller57802</t>
+  </si>
+  <si>
+    <t>Automation57802</t>
+  </si>
+  <si>
+    <t>controllerautomation57802@gmail.com</t>
+  </si>
+  <si>
+    <t>57802</t>
+  </si>
+  <si>
+    <t>Controller62324</t>
+  </si>
+  <si>
+    <t>Automation62324</t>
+  </si>
+  <si>
+    <t>controllerautomation62324@gmail.com</t>
+  </si>
+  <si>
+    <t>62324</t>
+  </si>
+  <si>
+    <t>Controller78047</t>
+  </si>
+  <si>
+    <t>Automation78047</t>
+  </si>
+  <si>
+    <t>controllerautomation78047@gmail.com</t>
+  </si>
+  <si>
+    <t>78047</t>
+  </si>
+  <si>
+    <t>Controller97459</t>
+  </si>
+  <si>
+    <t>Automation97459</t>
+  </si>
+  <si>
+    <t>controllerautomation97459@gmail.com</t>
+  </si>
+  <si>
+    <t>97459</t>
+  </si>
+  <si>
+    <t>Controller51803</t>
+  </si>
+  <si>
+    <t>Automation51803</t>
+  </si>
+  <si>
+    <t>controllerautomation51803@gmail.com</t>
+  </si>
+  <si>
+    <t>51803</t>
+  </si>
+  <si>
+    <t>Controller67974</t>
+  </si>
+  <si>
+    <t>Automation67974</t>
+  </si>
+  <si>
+    <t>controllerautomation67974@gmail.com</t>
+  </si>
+  <si>
+    <t>67974</t>
+  </si>
+  <si>
+    <t>Controller87666</t>
+  </si>
+  <si>
+    <t>Automation87666</t>
+  </si>
+  <si>
+    <t>controllerautomation87666@gmail.com</t>
+  </si>
+  <si>
+    <t>87666</t>
+  </si>
+  <si>
+    <t>Controller16480</t>
+  </si>
+  <si>
+    <t>Automation16480</t>
+  </si>
+  <si>
+    <t>controllerautomation16480@gmail.com</t>
+  </si>
+  <si>
+    <t>16480</t>
+  </si>
+  <si>
+    <t>Controller12533</t>
+  </si>
+  <si>
+    <t>Automation12533</t>
+  </si>
+  <si>
+    <t>controllerautomation12533@gmail.com</t>
+  </si>
+  <si>
+    <t>12533</t>
+  </si>
+  <si>
+    <t>Controller23544</t>
+  </si>
+  <si>
+    <t>Automation23544</t>
+  </si>
+  <si>
+    <t>controllerautomation23544@gmail.com</t>
+  </si>
+  <si>
+    <t>23544</t>
+  </si>
+  <si>
+    <t>Controller36449</t>
+  </si>
+  <si>
+    <t>Automation36449</t>
+  </si>
+  <si>
+    <t>controllerautomation36449@gmail.com</t>
+  </si>
+  <si>
+    <t>36449</t>
+  </si>
+  <si>
+    <t>Controller94654</t>
+  </si>
+  <si>
+    <t>Automation94654</t>
+  </si>
+  <si>
+    <t>controllerautomation94654@gmail.com</t>
+  </si>
+  <si>
+    <t>94654</t>
+  </si>
+  <si>
+    <t>Controller33228</t>
+  </si>
+  <si>
+    <t>Automation33228</t>
+  </si>
+  <si>
+    <t>controllerautomation33228@gmail.com</t>
+  </si>
+  <si>
+    <t>33228</t>
+  </si>
+  <si>
+    <t>Controller16378</t>
+  </si>
+  <si>
+    <t>Automation16378</t>
+  </si>
+  <si>
+    <t>controllerautomation16378@gmail.com</t>
+  </si>
+  <si>
+    <t>16378</t>
+  </si>
+  <si>
+    <t>Controller92436</t>
+  </si>
+  <si>
+    <t>Automation92436</t>
+  </si>
+  <si>
+    <t>controllerautomation92436@gmail.com</t>
+  </si>
+  <si>
+    <t>92436</t>
+  </si>
+  <si>
+    <t>Controller94809</t>
+  </si>
+  <si>
+    <t>Automation94809</t>
+  </si>
+  <si>
+    <t>controllerautomation94809@gmail.com</t>
+  </si>
+  <si>
+    <t>94809</t>
+  </si>
+  <si>
+    <t>Controller10331</t>
+  </si>
+  <si>
+    <t>Automation10331</t>
+  </si>
+  <si>
+    <t>controllerautomation10331@gmail.com</t>
+  </si>
+  <si>
+    <t>10331</t>
+  </si>
+  <si>
+    <t>Controller03781</t>
+  </si>
+  <si>
+    <t>Automation03781</t>
+  </si>
+  <si>
+    <t>controllerautomation03781@gmail.com</t>
+  </si>
+  <si>
+    <t>03781</t>
+  </si>
+  <si>
+    <t>Controller08936</t>
+  </si>
+  <si>
+    <t>Automation08936</t>
+  </si>
+  <si>
+    <t>controllerautomation08936@gmail.com</t>
+  </si>
+  <si>
+    <t>08936</t>
+  </si>
+  <si>
+    <t>Controller39298</t>
+  </si>
+  <si>
+    <t>Automation39298</t>
+  </si>
+  <si>
+    <t>controllerautomation39298@gmail.com</t>
+  </si>
+  <si>
+    <t>39298</t>
+  </si>
+  <si>
+    <t>Controller92304</t>
+  </si>
+  <si>
+    <t>Automation92304</t>
+  </si>
+  <si>
+    <t>controllerautomation92304@gmail.com</t>
+  </si>
+  <si>
+    <t>92304</t>
+  </si>
+  <si>
+    <t>Controller01737</t>
+  </si>
+  <si>
+    <t>Automation01737</t>
+  </si>
+  <si>
+    <t>controllerautomation01737@gmail.com</t>
+  </si>
+  <si>
+    <t>01737</t>
+  </si>
+  <si>
+    <t>Controller89338</t>
+  </si>
+  <si>
+    <t>Automation89338</t>
+  </si>
+  <si>
+    <t>controllerautomation89338@gmail.com</t>
+  </si>
+  <si>
+    <t>89338</t>
   </si>
 </sst>
 </file>
@@ -9065,422 +9425,422 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2757</v>
+        <v>2877</v>
       </c>
       <c r="B2" t="s">
-        <v>2758</v>
+        <v>2878</v>
       </c>
       <c r="C2" t="s">
-        <v>2759</v>
+        <v>2879</v>
       </c>
       <c r="D2" t="s">
-        <v>2760</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2761</v>
+        <v>2881</v>
       </c>
       <c r="B3" t="s">
-        <v>2762</v>
+        <v>2882</v>
       </c>
       <c r="C3" t="s">
-        <v>2763</v>
+        <v>2883</v>
       </c>
       <c r="D3" t="s">
-        <v>2764</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2765</v>
+        <v>2885</v>
       </c>
       <c r="B4" t="s">
-        <v>2766</v>
+        <v>2886</v>
       </c>
       <c r="C4" t="s">
-        <v>2767</v>
+        <v>2887</v>
       </c>
       <c r="D4" t="s">
-        <v>2768</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2769</v>
+        <v>2889</v>
       </c>
       <c r="B5" t="s">
-        <v>2770</v>
+        <v>2890</v>
       </c>
       <c r="C5" t="s">
-        <v>2771</v>
+        <v>2891</v>
       </c>
       <c r="D5" t="s">
-        <v>2772</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2773</v>
+        <v>2893</v>
       </c>
       <c r="B6" t="s">
-        <v>2774</v>
+        <v>2894</v>
       </c>
       <c r="C6" t="s">
-        <v>2775</v>
+        <v>2895</v>
       </c>
       <c r="D6" t="s">
-        <v>2776</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2777</v>
+        <v>2897</v>
       </c>
       <c r="B7" t="s">
-        <v>2778</v>
+        <v>2898</v>
       </c>
       <c r="C7" t="s">
-        <v>2779</v>
+        <v>2899</v>
       </c>
       <c r="D7" t="s">
-        <v>2780</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2781</v>
+        <v>2901</v>
       </c>
       <c r="B8" t="s">
-        <v>2782</v>
+        <v>2902</v>
       </c>
       <c r="C8" t="s">
-        <v>2783</v>
+        <v>2903</v>
       </c>
       <c r="D8" t="s">
-        <v>2784</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2785</v>
+        <v>2905</v>
       </c>
       <c r="B9" t="s">
-        <v>2786</v>
+        <v>2906</v>
       </c>
       <c r="C9" t="s">
-        <v>2787</v>
+        <v>2907</v>
       </c>
       <c r="D9" t="s">
-        <v>2788</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2789</v>
+        <v>2909</v>
       </c>
       <c r="B10" t="s">
-        <v>2790</v>
+        <v>2910</v>
       </c>
       <c r="C10" t="s">
-        <v>2791</v>
+        <v>2911</v>
       </c>
       <c r="D10" t="s">
-        <v>2792</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2793</v>
+        <v>2913</v>
       </c>
       <c r="B11" t="s">
-        <v>2794</v>
+        <v>2914</v>
       </c>
       <c r="C11" t="s">
-        <v>2795</v>
+        <v>2915</v>
       </c>
       <c r="D11" t="s">
-        <v>2796</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2797</v>
+        <v>2917</v>
       </c>
       <c r="B12" t="s">
-        <v>2798</v>
+        <v>2918</v>
       </c>
       <c r="C12" t="s">
-        <v>2799</v>
+        <v>2919</v>
       </c>
       <c r="D12" t="s">
-        <v>2800</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2801</v>
+        <v>2921</v>
       </c>
       <c r="B13" t="s">
-        <v>2802</v>
+        <v>2922</v>
       </c>
       <c r="C13" t="s">
-        <v>2803</v>
+        <v>2923</v>
       </c>
       <c r="D13" t="s">
-        <v>2804</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2805</v>
+        <v>2925</v>
       </c>
       <c r="B14" t="s">
-        <v>2806</v>
+        <v>2926</v>
       </c>
       <c r="C14" t="s">
-        <v>2807</v>
+        <v>2927</v>
       </c>
       <c r="D14" t="s">
-        <v>2808</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2809</v>
+        <v>2929</v>
       </c>
       <c r="B15" t="s">
-        <v>2810</v>
+        <v>2930</v>
       </c>
       <c r="C15" t="s">
-        <v>2811</v>
+        <v>2931</v>
       </c>
       <c r="D15" t="s">
-        <v>2812</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2813</v>
+        <v>2933</v>
       </c>
       <c r="B16" t="s">
-        <v>2814</v>
+        <v>2934</v>
       </c>
       <c r="C16" t="s">
-        <v>2815</v>
+        <v>2935</v>
       </c>
       <c r="D16" t="s">
-        <v>2816</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2817</v>
+        <v>2937</v>
       </c>
       <c r="B17" t="s">
-        <v>2818</v>
+        <v>2938</v>
       </c>
       <c r="C17" t="s">
-        <v>2819</v>
+        <v>2939</v>
       </c>
       <c r="D17" t="s">
-        <v>2820</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2821</v>
+        <v>2941</v>
       </c>
       <c r="B18" t="s">
-        <v>2822</v>
+        <v>2942</v>
       </c>
       <c r="C18" t="s">
-        <v>2823</v>
+        <v>2943</v>
       </c>
       <c r="D18" t="s">
-        <v>2824</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2825</v>
+        <v>2945</v>
       </c>
       <c r="B19" t="s">
-        <v>2826</v>
+        <v>2946</v>
       </c>
       <c r="C19" t="s">
-        <v>2827</v>
+        <v>2947</v>
       </c>
       <c r="D19" t="s">
-        <v>2828</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2829</v>
+        <v>2949</v>
       </c>
       <c r="B20" t="s">
-        <v>2830</v>
+        <v>2950</v>
       </c>
       <c r="C20" t="s">
-        <v>2831</v>
+        <v>2951</v>
       </c>
       <c r="D20" t="s">
-        <v>2832</v>
+        <v>2952</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>2833</v>
+        <v>2953</v>
       </c>
       <c r="B21" t="s">
-        <v>2834</v>
+        <v>2954</v>
       </c>
       <c r="C21" t="s">
-        <v>2835</v>
+        <v>2955</v>
       </c>
       <c r="D21" t="s">
-        <v>2836</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>2837</v>
+        <v>2957</v>
       </c>
       <c r="B22" t="s">
-        <v>2838</v>
+        <v>2958</v>
       </c>
       <c r="C22" t="s">
-        <v>2839</v>
+        <v>2959</v>
       </c>
       <c r="D22" t="s">
-        <v>2840</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>2841</v>
+        <v>2961</v>
       </c>
       <c r="B23" t="s">
-        <v>2842</v>
+        <v>2962</v>
       </c>
       <c r="C23" t="s">
-        <v>2843</v>
+        <v>2963</v>
       </c>
       <c r="D23" t="s">
-        <v>2844</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>2845</v>
+        <v>2965</v>
       </c>
       <c r="B24" t="s">
-        <v>2846</v>
+        <v>2966</v>
       </c>
       <c r="C24" t="s">
-        <v>2847</v>
+        <v>2967</v>
       </c>
       <c r="D24" t="s">
-        <v>2848</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>2849</v>
+        <v>2969</v>
       </c>
       <c r="B25" t="s">
-        <v>2850</v>
+        <v>2970</v>
       </c>
       <c r="C25" t="s">
-        <v>2851</v>
+        <v>2971</v>
       </c>
       <c r="D25" t="s">
-        <v>2852</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>2853</v>
+        <v>2973</v>
       </c>
       <c r="B26" t="s">
-        <v>2854</v>
+        <v>2974</v>
       </c>
       <c r="C26" t="s">
-        <v>2855</v>
+        <v>2975</v>
       </c>
       <c r="D26" t="s">
-        <v>2856</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>2857</v>
+        <v>2977</v>
       </c>
       <c r="B27" t="s">
-        <v>2858</v>
+        <v>2978</v>
       </c>
       <c r="C27" t="s">
-        <v>2859</v>
+        <v>2979</v>
       </c>
       <c r="D27" t="s">
-        <v>2860</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>2861</v>
+        <v>2981</v>
       </c>
       <c r="B28" t="s">
-        <v>2862</v>
+        <v>2982</v>
       </c>
       <c r="C28" t="s">
-        <v>2863</v>
+        <v>2983</v>
       </c>
       <c r="D28" t="s">
-        <v>2864</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>2865</v>
+        <v>2985</v>
       </c>
       <c r="B29" t="s">
-        <v>2866</v>
+        <v>2986</v>
       </c>
       <c r="C29" t="s">
-        <v>2867</v>
+        <v>2987</v>
       </c>
       <c r="D29" t="s">
-        <v>2868</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>2869</v>
+        <v>2989</v>
       </c>
       <c r="B30" t="s">
-        <v>2870</v>
+        <v>2990</v>
       </c>
       <c r="C30" t="s">
-        <v>2871</v>
+        <v>2991</v>
       </c>
       <c r="D30" t="s">
-        <v>2872</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2873</v>
+        <v>2993</v>
       </c>
       <c r="B31" t="s">
-        <v>2874</v>
+        <v>2994</v>
       </c>
       <c r="C31" t="s">
-        <v>2875</v>
+        <v>2995</v>
       </c>
       <c r="D31" t="s">
-        <v>2876</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="32"/>

</xml_diff>